<commit_message>
Commiting Experiments on Dataset
</commit_message>
<xml_diff>
--- a/ExperimentReport/DataSet-2/Experiment Report.xlsx
+++ b/ExperimentReport/DataSet-2/Experiment Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C49F26D-CB4E-4382-A71B-C6ED3465C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F828E097-5800-44B4-B5F8-34471A37FC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Experiment Github URL</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-2/Exp-18</t>
+  </si>
+  <si>
+    <t>https://github.com/GurunagSai/neocortexapi-classification/tree/GurunagSai/ExperimentReport/DataSet-2/Exp-17</t>
   </si>
 </sst>
 </file>
@@ -217,6 +223,15 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -226,21 +241,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,644 +530,704 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="65.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="59" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="65.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="5" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>30</v>
       </c>
-      <c r="E3" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="E3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="2">
         <v>0.1</v>
       </c>
-      <c r="G3" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
         <v>30</v>
       </c>
-      <c r="E4" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="2">
         <v>0.15</v>
       </c>
-      <c r="G4" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
         <v>30</v>
       </c>
-      <c r="E5" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="E5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2">
         <v>0.2</v>
       </c>
-      <c r="G5" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>30</v>
       </c>
-      <c r="E6" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="7">
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.25</v>
       </c>
-      <c r="G6" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H6" s="7" t="s">
+      <c r="G6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>20</v>
       </c>
-      <c r="E7" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="E7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="2">
         <v>0.1</v>
       </c>
-      <c r="G7" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H7" s="7" t="s">
+      <c r="G7" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
         <v>10</v>
       </c>
-      <c r="E8" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="2">
         <v>0.1</v>
       </c>
-      <c r="G8" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
         <v>10</v>
       </c>
-      <c r="E9" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="E9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.15</v>
       </c>
-      <c r="G9" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="G9" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <v>10</v>
       </c>
-      <c r="E10" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="2">
         <v>0.2</v>
       </c>
-      <c r="G10" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="8" t="s">
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
-        <v>1</v>
-      </c>
-      <c r="C11" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="7">
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="2">
         <v>0.1</v>
       </c>
-      <c r="G11" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="2">
         <v>0.2</v>
       </c>
-      <c r="G12" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="8" t="s">
+      <c r="I12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
         <v>10</v>
       </c>
-      <c r="E13" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="E13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="2">
         <v>10</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="8" t="s">
+      <c r="I13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
         <v>10</v>
       </c>
-      <c r="E14" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="E14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="2">
         <v>0.1</v>
       </c>
-      <c r="G14" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H14" s="7" t="s">
+      <c r="G14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" s="8" t="s">
+      <c r="I14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="7">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
         <v>20</v>
       </c>
-      <c r="E15" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="E15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="2">
         <v>0.2</v>
       </c>
-      <c r="G15" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H15" s="7" t="s">
+      <c r="G15" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J15" s="8" t="s">
+      <c r="I15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7">
+      <c r="A16" s="2">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7">
+      <c r="C16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
         <v>5</v>
       </c>
-      <c r="E16" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="7">
+      <c r="E16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="2">
         <v>10</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="8" t="s">
+      <c r="I16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
         <v>3</v>
       </c>
-      <c r="E17" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="E17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="2">
         <v>0.1</v>
       </c>
-      <c r="G17" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="G17" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="8" t="s">
+      <c r="I17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
         <v>3</v>
       </c>
-      <c r="E18" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="E18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="2">
         <v>0.15</v>
       </c>
-      <c r="G18" s="7">
-        <v>-1</v>
-      </c>
-      <c r="H18" s="7" t="s">
+      <c r="G18" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="8" t="s">
+      <c r="I18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>30</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>18</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1188,8 +1254,10 @@
     <hyperlink ref="J16" r:id="rId14" xr:uid="{CDC22AB1-6CD5-4A49-8EC5-0E8E9B840729}"/>
     <hyperlink ref="J17" r:id="rId15" xr:uid="{0075321B-4373-44C0-87C9-B2D7D79307CF}"/>
     <hyperlink ref="J18" r:id="rId16" xr:uid="{BEA07F0A-FD0D-497B-933D-3E0C9A5E0A8A}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{9474A528-176C-4F3A-9035-9A4FE81CD42A}"/>
+    <hyperlink ref="J19" r:id="rId18" xr:uid="{371AE9A6-EAB8-4D30-9172-FA31F09835AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>